<commit_message>
Updated mint- and transfergasconsumption data of ERC72F contract
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C3D0B-22A6-4EA2-9EC1-DAE45B6845F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B17C346-0A0F-4160-B01F-ED3E0BAF3659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled" sheetId="1" r:id="rId1"/>
@@ -607,13 +607,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74639</c:v>
+                  <c:v>74559</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>305706</c:v>
+                  <c:v>305347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2616839</c:v>
+                  <c:v>2613690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,7 +1372,7 @@
                   <c:v>92881</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64164</c:v>
+                  <c:v>64129</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>85991</c:v>
@@ -1472,7 +1472,7 @@
                   <c:v>442480</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197126</c:v>
+                  <c:v>196776</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>256208</c:v>
@@ -2014,7 +2014,7 @@
                   <c:v>557550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201926</c:v>
+                  <c:v>201576</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>367550</c:v>
@@ -2114,7 +2114,7 @@
                   <c:v>2939851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1131142</c:v>
+                  <c:v>1129392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2116229</c:v>
@@ -2665,7 +2665,7 @@
                   <c:v>67205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59170</c:v>
+                  <c:v>59135</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52228</c:v>
@@ -3227,7 +3227,7 @@
                   <c:v>88187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64252</c:v>
+                  <c:v>64217</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104804</c:v>
@@ -3327,7 +3327,7 @@
                   <c:v>461387</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197368</c:v>
+                  <c:v>197018</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>264289</c:v>
@@ -3919,7 +3919,7 @@
                   <c:v>485934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>202450</c:v>
+                  <c:v>202100</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>935546</c:v>
@@ -4019,7 +4019,7 @@
                   <c:v>2567476</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1131142</c:v>
+                  <c:v>1129392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3747936</c:v>
@@ -4654,13 +4654,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73926</c:v>
+                  <c:v>73879</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300241</c:v>
+                  <c:v>300086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2563854</c:v>
+                  <c:v>2562619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5388,7 +5388,7 @@
                   <c:v>67419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59340</c:v>
+                  <c:v>59305</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52673</c:v>
@@ -5954,7 +5954,7 @@
                   <c:v>92813</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64140</c:v>
+                  <c:v>64105</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>86014</c:v>
@@ -6054,7 +6054,7 @@
                   <c:v>442196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196886</c:v>
+                  <c:v>196536</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>256186</c:v>
@@ -6646,7 +6646,7 @@
                   <c:v>557266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201686</c:v>
+                  <c:v>201336</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>367528</c:v>
@@ -6746,7 +6746,7 @@
                   <c:v>2938607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1129942</c:v>
+                  <c:v>1128192</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2116185</c:v>
@@ -7288,7 +7288,7 @@
                   <c:v>67204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59146</c:v>
+                  <c:v>59111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52251</c:v>
@@ -7827,7 +7827,7 @@
                   <c:v>68519</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60198</c:v>
+                  <c:v>60149</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53592</c:v>
@@ -8352,7 +8352,7 @@
                   <c:v>88186</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64228</c:v>
+                  <c:v>64193</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104827</c:v>
@@ -8452,7 +8452,7 @@
                   <c:v>461103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197128</c:v>
+                  <c:v>196778</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>264245</c:v>
@@ -9007,7 +9007,7 @@
                   <c:v>485650</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>202210</c:v>
+                  <c:v>201860</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>935502</c:v>
@@ -9107,7 +9107,7 @@
                   <c:v>2566276</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1129942</c:v>
+                  <c:v>1128192</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3747892</c:v>
@@ -9735,13 +9735,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74639</c:v>
+                  <c:v>74559</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>305706</c:v>
+                  <c:v>305347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2616839</c:v>
+                  <c:v>2613690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10541,13 +10541,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73938</c:v>
+                  <c:v>73891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300361</c:v>
+                  <c:v>300206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2565054</c:v>
+                  <c:v>2563819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11356,13 +11356,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73926</c:v>
+                  <c:v>73879</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300241</c:v>
+                  <c:v>300086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2563854</c:v>
+                  <c:v>2562619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12116,7 +12116,7 @@
                   <c:v>92881</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64164</c:v>
+                  <c:v>64129</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>85991</c:v>
@@ -12216,7 +12216,7 @@
                   <c:v>442480</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197126</c:v>
+                  <c:v>196776</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>256208</c:v>
@@ -12763,7 +12763,7 @@
                   <c:v>94074</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64998</c:v>
+                  <c:v>64949</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>86980</c:v>
@@ -12863,7 +12863,7 @@
                   <c:v>455841</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207702</c:v>
+                  <c:v>207212</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>269980</c:v>
@@ -13437,7 +13437,7 @@
                   <c:v>68519</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60198</c:v>
+                  <c:v>60149</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53592</c:v>
@@ -13970,7 +13970,7 @@
                   <c:v>67487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59364</c:v>
+                  <c:v>59329</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52650</c:v>
@@ -14487,7 +14487,7 @@
                   <c:v>571716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212502</c:v>
+                  <c:v>212012</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>381566</c:v>
@@ -14587,7 +14587,7 @@
                   <c:v>3087077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1274268</c:v>
+                  <c:v>1271818</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2304705</c:v>
@@ -15129,7 +15129,7 @@
                   <c:v>94074</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64998</c:v>
+                  <c:v>64949</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>86980</c:v>
@@ -15229,7 +15229,7 @@
                   <c:v>455841</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207702</c:v>
+                  <c:v>207212</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>269980</c:v>
@@ -15788,7 +15788,7 @@
                   <c:v>557550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201926</c:v>
+                  <c:v>201576</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>367550</c:v>
@@ -15888,7 +15888,7 @@
                   <c:v>2939851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1131142</c:v>
+                  <c:v>1129392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2116229</c:v>
@@ -16454,7 +16454,7 @@
                   <c:v>67419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59340</c:v>
+                  <c:v>59305</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52673</c:v>
@@ -16997,7 +16997,7 @@
                   <c:v>92813</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64140</c:v>
+                  <c:v>64105</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>86014</c:v>
@@ -17097,7 +17097,7 @@
                   <c:v>442196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196886</c:v>
+                  <c:v>196536</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>256186</c:v>
@@ -17666,7 +17666,7 @@
                   <c:v>557266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201686</c:v>
+                  <c:v>201336</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>367528</c:v>
@@ -17766,7 +17766,7 @@
                   <c:v>2938607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1129942</c:v>
+                  <c:v>1128192</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2116185</c:v>
@@ -18312,7 +18312,7 @@
                   <c:v>68287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60054</c:v>
+                  <c:v>60005</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53178</c:v>
@@ -18833,7 +18833,7 @@
                   <c:v>89349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65216</c:v>
+                  <c:v>65167</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>106482</c:v>
@@ -18933,7 +18933,7 @@
                   <c:v>475836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209434</c:v>
+                  <c:v>208944</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>280869</c:v>
@@ -19479,7 +19479,7 @@
                   <c:v>500060</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214596</c:v>
+                  <c:v>214106</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1011433</c:v>
@@ -19579,7 +19579,7 @@
                   <c:v>2720502</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1274268</c:v>
+                  <c:v>1271818</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4187763</c:v>
@@ -20131,7 +20131,7 @@
                   <c:v>67205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59170</c:v>
+                  <c:v>59135</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52228</c:v>
@@ -20670,7 +20670,7 @@
                   <c:v>88187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64252</c:v>
+                  <c:v>64217</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104804</c:v>
@@ -20770,7 +20770,7 @@
                   <c:v>461387</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197368</c:v>
+                  <c:v>197018</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>264289</c:v>
@@ -21339,7 +21339,7 @@
                   <c:v>485934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>202450</c:v>
+                  <c:v>202100</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>935546</c:v>
@@ -21439,7 +21439,7 @@
                   <c:v>2567476</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1131142</c:v>
+                  <c:v>1129392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3747936</c:v>
@@ -21986,7 +21986,7 @@
                   <c:v>571716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212502</c:v>
+                  <c:v>212012</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>381566</c:v>
@@ -22086,7 +22086,7 @@
                   <c:v>3087077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1274268</c:v>
+                  <c:v>1271818</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2304705</c:v>
@@ -22630,7 +22630,7 @@
                   <c:v>67204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59146</c:v>
+                  <c:v>59111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52251</c:v>
@@ -23152,7 +23152,7 @@
                   <c:v>88186</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64228</c:v>
+                  <c:v>64193</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104827</c:v>
@@ -23252,7 +23252,7 @@
                   <c:v>461103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197128</c:v>
+                  <c:v>196778</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>264245</c:v>
@@ -23804,7 +23804,7 @@
                   <c:v>485650</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>202210</c:v>
+                  <c:v>201860</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>935502</c:v>
@@ -23904,7 +23904,7 @@
                   <c:v>2566276</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1129942</c:v>
+                  <c:v>1128192</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3747892</c:v>
@@ -24450,7 +24450,7 @@
                   <c:v>68287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60054</c:v>
+                  <c:v>60005</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53178</c:v>
@@ -24994,7 +24994,7 @@
                   <c:v>89349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65216</c:v>
+                  <c:v>65167</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>106482</c:v>
@@ -25094,7 +25094,7 @@
                   <c:v>475836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209434</c:v>
+                  <c:v>208944</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>280869</c:v>
@@ -25663,7 +25663,7 @@
                   <c:v>500060</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214596</c:v>
+                  <c:v>214106</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1011433</c:v>
@@ -25763,7 +25763,7 @@
                   <c:v>2720502</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1274268</c:v>
+                  <c:v>1271818</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4187763</c:v>
@@ -26394,13 +26394,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73938</c:v>
+                  <c:v>73891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300361</c:v>
+                  <c:v>300206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2565054</c:v>
+                  <c:v>2563819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27128,7 +27128,7 @@
                   <c:v>67487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59364</c:v>
+                  <c:v>59329</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52650</c:v>
@@ -51763,8 +51763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0F01C6-732F-4ED7-AFD2-583E8DD3800A}">
   <dimension ref="C3:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="R22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y31" sqref="Y31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -51828,13 +51828,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>74639</v>
+        <v>74559</v>
       </c>
       <c r="K4" s="4">
-        <v>305706</v>
+        <v>305347</v>
       </c>
       <c r="L4" s="4">
-        <v>2616839</v>
+        <v>2613690</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -51867,10 +51867,10 @@
         <v>3</v>
       </c>
       <c r="J5" s="4">
-        <v>60198</v>
+        <v>60149</v>
       </c>
       <c r="K5" s="5">
-        <v>64998</v>
+        <v>64949</v>
       </c>
       <c r="L5" s="4"/>
       <c r="O5" s="2" t="s">
@@ -51878,15 +51878,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>74639</v>
+        <v>74559</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>305706</v>
+        <v>305347</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2616839</v>
+        <v>2613690</v>
       </c>
     </row>
     <row r="6" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -51904,10 +51904,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>60054</v>
+        <v>60005</v>
       </c>
       <c r="K6" s="5">
-        <v>65216</v>
+        <v>65167</v>
       </c>
       <c r="L6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -51942,10 +51942,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
-        <v>207702</v>
+        <v>207212</v>
       </c>
       <c r="L7" s="5">
-        <v>212502</v>
+        <v>212012</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>11</v>
@@ -51976,10 +51976,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
-        <v>209434</v>
+        <v>208944</v>
       </c>
       <c r="L8" s="5">
-        <v>214596</v>
+        <v>214106</v>
       </c>
     </row>
     <row r="9" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -51997,7 +51997,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
-        <v>1260783</v>
+        <v>1258333</v>
       </c>
     </row>
     <row r="10" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52015,7 +52015,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>1274268</v>
+        <v>1271818</v>
       </c>
     </row>
     <row r="11" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52125,7 +52125,7 @@
       </c>
       <c r="P15" s="4">
         <f>J5</f>
-        <v>60198</v>
+        <v>60149</v>
       </c>
       <c r="Q15"/>
       <c r="R15"/>
@@ -52134,7 +52134,7 @@
       </c>
       <c r="Z15" s="4">
         <f>J6</f>
-        <v>60054</v>
+        <v>60005</v>
       </c>
     </row>
     <row r="16" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52347,22 +52347,22 @@
       </c>
       <c r="P25" s="7">
         <f>K5</f>
-        <v>64998</v>
+        <v>64949</v>
       </c>
       <c r="Q25" s="4">
         <f>K7</f>
-        <v>207702</v>
+        <v>207212</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z25" s="7">
         <f>K6</f>
-        <v>65216</v>
+        <v>65167</v>
       </c>
       <c r="AA25" s="4">
         <f>K8</f>
-        <v>209434</v>
+        <v>208944</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52463,22 +52463,22 @@
       </c>
       <c r="P35" s="7">
         <f>L7</f>
-        <v>212502</v>
+        <v>212012</v>
       </c>
       <c r="Q35" s="4">
         <f>L10</f>
-        <v>1274268</v>
+        <v>1271818</v>
       </c>
       <c r="Y35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z35" s="7">
         <f>L8</f>
-        <v>214596</v>
+        <v>214106</v>
       </c>
       <c r="AA35" s="4">
         <f>L10</f>
-        <v>1274268</v>
+        <v>1271818</v>
       </c>
     </row>
     <row r="36" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52540,8 +52540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A4B072-C80B-4A23-A0B3-8E3559BB66E3}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="W25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52604,13 +52604,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>73938</v>
+        <v>73891</v>
       </c>
       <c r="K4" s="4">
-        <v>300361</v>
+        <v>300206</v>
       </c>
       <c r="L4" s="4">
-        <v>2565054</v>
+        <v>2563819</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -52643,10 +52643,10 @@
         <v>3</v>
       </c>
       <c r="J5" s="4">
-        <v>59364</v>
+        <v>59329</v>
       </c>
       <c r="K5" s="5">
-        <v>64164</v>
+        <v>64129</v>
       </c>
       <c r="L5" s="4"/>
       <c r="O5" s="2" t="s">
@@ -52654,15 +52654,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>73938</v>
+        <v>73891</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>300361</v>
+        <v>300206</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2565054</v>
+        <v>2563819</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52680,10 +52680,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>59170</v>
+        <v>59135</v>
       </c>
       <c r="K6" s="5">
-        <v>64252</v>
+        <v>64217</v>
       </c>
       <c r="L6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -52718,10 +52718,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
-        <v>197126</v>
+        <v>196776</v>
       </c>
       <c r="L7" s="5">
-        <v>201926</v>
+        <v>201576</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>11</v>
@@ -52752,10 +52752,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
-        <v>197368</v>
+        <v>197018</v>
       </c>
       <c r="L8" s="5">
-        <v>202450</v>
+        <v>202100</v>
       </c>
     </row>
     <row r="9" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52773,7 +52773,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
-        <v>1131507</v>
+        <v>1129757</v>
       </c>
     </row>
     <row r="10" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52791,7 +52791,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>1131142</v>
+        <v>1129392</v>
       </c>
     </row>
     <row r="11" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52900,7 +52900,7 @@
       </c>
       <c r="P15" s="4">
         <f>J5</f>
-        <v>59364</v>
+        <v>59329</v>
       </c>
       <c r="Q15"/>
       <c r="Y15" s="2" t="s">
@@ -52908,7 +52908,7 @@
       </c>
       <c r="Z15" s="4">
         <f>J6</f>
-        <v>59170</v>
+        <v>59135</v>
       </c>
       <c r="AA15"/>
     </row>
@@ -53127,22 +53127,22 @@
       </c>
       <c r="P25" s="7">
         <f>K5</f>
-        <v>64164</v>
+        <v>64129</v>
       </c>
       <c r="Q25" s="4">
         <f>K7</f>
-        <v>197126</v>
+        <v>196776</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z25" s="7">
         <f>K6</f>
-        <v>64252</v>
+        <v>64217</v>
       </c>
       <c r="AA25" s="4">
         <f>K8</f>
-        <v>197368</v>
+        <v>197018</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53258,22 +53258,22 @@
       </c>
       <c r="P35" s="7">
         <f>L7</f>
-        <v>201926</v>
+        <v>201576</v>
       </c>
       <c r="Q35" s="4">
         <f>L10</f>
-        <v>1131142</v>
+        <v>1129392</v>
       </c>
       <c r="Y35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z35" s="7">
         <f>L8</f>
-        <v>202450</v>
+        <v>202100</v>
       </c>
       <c r="AA35" s="4">
         <f>L10</f>
-        <v>1131142</v>
+        <v>1129392</v>
       </c>
     </row>
     <row r="36" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53334,8 +53334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE8ECB1-BB77-4268-B40B-9743FF1BA452}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="W25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53398,13 +53398,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>73926</v>
+        <v>73879</v>
       </c>
       <c r="K4" s="4">
-        <v>300241</v>
+        <v>300086</v>
       </c>
       <c r="L4" s="4">
-        <v>2563854</v>
+        <v>2562619</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -53437,10 +53437,10 @@
         <v>3</v>
       </c>
       <c r="J5" s="4">
-        <v>59340</v>
+        <v>59305</v>
       </c>
       <c r="K5" s="5">
-        <v>64140</v>
+        <v>64105</v>
       </c>
       <c r="L5" s="4"/>
       <c r="O5" s="2" t="s">
@@ -53448,15 +53448,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>73926</v>
+        <v>73879</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>300241</v>
+        <v>300086</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2563854</v>
+        <v>2562619</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53474,10 +53474,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>59146</v>
+        <v>59111</v>
       </c>
       <c r="K6" s="5">
-        <v>64228</v>
+        <v>64193</v>
       </c>
       <c r="L6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -53512,10 +53512,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
-        <v>196886</v>
+        <v>196536</v>
       </c>
       <c r="L7" s="5">
-        <v>201686</v>
+        <v>201336</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>11</v>
@@ -53546,10 +53546,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
-        <v>197128</v>
+        <v>196778</v>
       </c>
       <c r="L8" s="5">
-        <v>202210</v>
+        <v>201860</v>
       </c>
     </row>
     <row r="9" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53567,7 +53567,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
-        <v>1130307</v>
+        <v>1128557</v>
       </c>
     </row>
     <row r="10" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53585,7 +53585,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>1129942</v>
+        <v>1128192</v>
       </c>
     </row>
     <row r="11" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53694,7 +53694,7 @@
       </c>
       <c r="P15" s="4">
         <f>J5</f>
-        <v>59340</v>
+        <v>59305</v>
       </c>
       <c r="Q15"/>
       <c r="Y15" s="2" t="s">
@@ -53702,7 +53702,7 @@
       </c>
       <c r="Z15" s="4">
         <f>J6</f>
-        <v>59146</v>
+        <v>59111</v>
       </c>
       <c r="AA15"/>
     </row>
@@ -53921,22 +53921,22 @@
       </c>
       <c r="P25" s="7">
         <f>K5</f>
-        <v>64140</v>
+        <v>64105</v>
       </c>
       <c r="Q25" s="4">
         <f>K7</f>
-        <v>196886</v>
+        <v>196536</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z25" s="7">
         <f>K6</f>
-        <v>64228</v>
+        <v>64193</v>
       </c>
       <c r="AA25" s="4">
         <f>K8</f>
-        <v>197128</v>
+        <v>196778</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54052,22 +54052,22 @@
       </c>
       <c r="P35" s="7">
         <f>L7</f>
-        <v>201686</v>
+        <v>201336</v>
       </c>
       <c r="Q35" s="4">
         <f>L10</f>
-        <v>1129942</v>
+        <v>1128192</v>
       </c>
       <c r="Y35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z35" s="7">
         <f>L8</f>
-        <v>202210</v>
+        <v>201860</v>
       </c>
       <c r="AA35" s="4">
         <f>L10</f>
-        <v>1129942</v>
+        <v>1128192</v>
       </c>
     </row>
     <row r="36" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54128,8 +54128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A3369B-EFF2-4697-8F13-FA8E3F78DF3C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BM104" sqref="BM104"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated ERC721F data with latest OpenZeppelin version
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC782AF-7564-4380-A1A1-6117AB964B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B737971-91EE-42E2-A971-F7970E9D7D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled" sheetId="1" r:id="rId1"/>
@@ -607,13 +607,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74559</c:v>
+                  <c:v>74788</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>305347</c:v>
+                  <c:v>307637</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2613690</c:v>
+                  <c:v>2636590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,7 +1372,7 @@
                   <c:v>92881</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64129</c:v>
+                  <c:v>62039</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>85719</c:v>
@@ -1472,7 +1472,7 @@
                   <c:v>442480</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196776</c:v>
+                  <c:v>175741</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>247368</c:v>
@@ -2014,7 +2014,7 @@
                   <c:v>557550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201576</c:v>
+                  <c:v>180541</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>358710</c:v>
@@ -2114,7 +2114,7 @@
                   <c:v>2939851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1105167</c:v>
+                  <c:v>996992</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1936029</c:v>
@@ -2665,7 +2665,7 @@
                   <c:v>67468</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59398</c:v>
+                  <c:v>57308</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52403</c:v>
@@ -3227,7 +3227,7 @@
                   <c:v>88168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64198</c:v>
+                  <c:v>62108</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104737</c:v>
@@ -3327,7 +3327,7 @@
                   <c:v>460624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196255</c:v>
+                  <c:v>175220</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>255878</c:v>
@@ -3919,7 +3919,7 @@
                   <c:v>484889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201055</c:v>
+                  <c:v>180020</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>927901</c:v>
@@ -4019,7 +4019,7 @@
                   <c:v>2543251</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1105167</c:v>
+                  <c:v>996992</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3554711</c:v>
@@ -4654,13 +4654,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73879</c:v>
+                  <c:v>74049</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300086</c:v>
+                  <c:v>301786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2562619</c:v>
+                  <c:v>2579619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5388,7 +5388,7 @@
                   <c:v>67419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59305</c:v>
+                  <c:v>57227</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52401</c:v>
@@ -5954,7 +5954,7 @@
                   <c:v>92813</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64105</c:v>
+                  <c:v>62027</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>85742</c:v>
@@ -6054,7 +6054,7 @@
                   <c:v>442196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196536</c:v>
+                  <c:v>175621</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>247324</c:v>
@@ -6646,7 +6646,7 @@
                   <c:v>557266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201336</c:v>
+                  <c:v>180421</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>358666</c:v>
@@ -6746,7 +6746,7 @@
                   <c:v>2938607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1103967</c:v>
+                  <c:v>996392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1935985</c:v>
@@ -7288,7 +7288,7 @@
                   <c:v>67467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59374</c:v>
+                  <c:v>57296</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52426</c:v>
@@ -7827,7 +7827,7 @@
                   <c:v>68519</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60149</c:v>
+                  <c:v>58022</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53288</c:v>
@@ -8352,7 +8352,7 @@
                   <c:v>88167</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64174</c:v>
+                  <c:v>62096</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104760</c:v>
@@ -8452,7 +8452,7 @@
                   <c:v>460340</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196015</c:v>
+                  <c:v>175100</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>255834</c:v>
@@ -9007,7 +9007,7 @@
                   <c:v>484605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200815</c:v>
+                  <c:v>179900</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>927857</c:v>
@@ -9107,7 +9107,7 @@
                   <c:v>2542051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1103967</c:v>
+                  <c:v>996392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3554667</c:v>
@@ -9735,13 +9735,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74559</c:v>
+                  <c:v>74788</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>305347</c:v>
+                  <c:v>307637</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2613690</c:v>
+                  <c:v>2636590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10541,13 +10541,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73891</c:v>
+                  <c:v>74061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300206</c:v>
+                  <c:v>301906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2563819</c:v>
+                  <c:v>2580819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11356,13 +11356,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73879</c:v>
+                  <c:v>74049</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300086</c:v>
+                  <c:v>301786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2562619</c:v>
+                  <c:v>2579619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12116,7 +12116,7 @@
                   <c:v>92881</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64129</c:v>
+                  <c:v>62039</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>85719</c:v>
@@ -12216,7 +12216,7 @@
                   <c:v>442480</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196776</c:v>
+                  <c:v>175741</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>247368</c:v>
@@ -12763,7 +12763,7 @@
                   <c:v>94074</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64949</c:v>
+                  <c:v>62822</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>86676</c:v>
@@ -12863,7 +12863,7 @@
                   <c:v>455841</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207212</c:v>
+                  <c:v>187607</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>260100</c:v>
@@ -13437,7 +13437,7 @@
                   <c:v>68519</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60149</c:v>
+                  <c:v>58022</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53288</c:v>
@@ -13970,7 +13970,7 @@
                   <c:v>67487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59329</c:v>
+                  <c:v>57239</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52378</c:v>
@@ -14487,7 +14487,7 @@
                   <c:v>571716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212012</c:v>
+                  <c:v>192407</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>371686</c:v>
@@ -14587,7 +14587,7 @@
                   <c:v>3087077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1267993</c:v>
+                  <c:v>1206968</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2103305</c:v>
@@ -15129,7 +15129,7 @@
                   <c:v>94074</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64949</c:v>
+                  <c:v>62822</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>86676</c:v>
@@ -15229,7 +15229,7 @@
                   <c:v>455841</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207212</c:v>
+                  <c:v>187607</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>260100</c:v>
@@ -15788,7 +15788,7 @@
                   <c:v>557550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201576</c:v>
+                  <c:v>180541</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>358710</c:v>
@@ -15888,7 +15888,7 @@
                   <c:v>2939851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1105167</c:v>
+                  <c:v>996992</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1936029</c:v>
@@ -16454,7 +16454,7 @@
                   <c:v>67419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59305</c:v>
+                  <c:v>57227</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52401</c:v>
@@ -16997,7 +16997,7 @@
                   <c:v>92813</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64105</c:v>
+                  <c:v>62027</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>85742</c:v>
@@ -17097,7 +17097,7 @@
                   <c:v>442196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196536</c:v>
+                  <c:v>175621</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>247324</c:v>
@@ -17666,7 +17666,7 @@
                   <c:v>557266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201336</c:v>
+                  <c:v>180421</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>358666</c:v>
@@ -17766,7 +17766,7 @@
                   <c:v>2938607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1103967</c:v>
+                  <c:v>996392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1935985</c:v>
@@ -18312,7 +18312,7 @@
                   <c:v>68646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60364</c:v>
+                  <c:v>58237</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53459</c:v>
@@ -18833,7 +18833,7 @@
                   <c:v>89346</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65164</c:v>
+                  <c:v>63037</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>106591</c:v>
@@ -18933,7 +18933,7 @@
                   <c:v>476033</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209141</c:v>
+                  <c:v>189536</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>272852</c:v>
@@ -19479,7 +19479,7 @@
                   <c:v>499895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>213941</c:v>
+                  <c:v>194336</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1026068</c:v>
@@ -19579,7 +19579,7 @@
                   <c:v>2716677</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1267993</c:v>
+                  <c:v>1206968</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4081938</c:v>
@@ -20131,7 +20131,7 @@
                   <c:v>67468</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59398</c:v>
+                  <c:v>57308</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52403</c:v>
@@ -20670,7 +20670,7 @@
                   <c:v>88168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64198</c:v>
+                  <c:v>62108</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104737</c:v>
@@ -20770,7 +20770,7 @@
                   <c:v>460624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196255</c:v>
+                  <c:v>175220</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>255878</c:v>
@@ -21339,7 +21339,7 @@
                   <c:v>484889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201055</c:v>
+                  <c:v>180020</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>927901</c:v>
@@ -21439,7 +21439,7 @@
                   <c:v>2543251</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1105167</c:v>
+                  <c:v>996992</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3554711</c:v>
@@ -21986,7 +21986,7 @@
                   <c:v>571716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212012</c:v>
+                  <c:v>192407</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>371686</c:v>
@@ -22086,7 +22086,7 @@
                   <c:v>3087077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1267993</c:v>
+                  <c:v>1206968</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2103305</c:v>
@@ -22630,7 +22630,7 @@
                   <c:v>67467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59374</c:v>
+                  <c:v>57296</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52426</c:v>
@@ -23152,7 +23152,7 @@
                   <c:v>88167</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64174</c:v>
+                  <c:v>62096</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104760</c:v>
@@ -23252,7 +23252,7 @@
                   <c:v>460340</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196015</c:v>
+                  <c:v>175100</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>255834</c:v>
@@ -23804,7 +23804,7 @@
                   <c:v>484605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200815</c:v>
+                  <c:v>179900</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>927857</c:v>
@@ -23904,7 +23904,7 @@
                   <c:v>2542051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1103967</c:v>
+                  <c:v>996392</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3554667</c:v>
@@ -24450,7 +24450,7 @@
                   <c:v>68646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60364</c:v>
+                  <c:v>58237</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53459</c:v>
@@ -24994,7 +24994,7 @@
                   <c:v>89346</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65164</c:v>
+                  <c:v>63037</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>106591</c:v>
@@ -25094,7 +25094,7 @@
                   <c:v>476033</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209141</c:v>
+                  <c:v>189536</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>272852</c:v>
@@ -25663,7 +25663,7 @@
                   <c:v>499895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>213941</c:v>
+                  <c:v>194336</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1026068</c:v>
@@ -25763,7 +25763,7 @@
                   <c:v>2716677</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1267993</c:v>
+                  <c:v>1206968</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4081938</c:v>
@@ -26394,13 +26394,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73891</c:v>
+                  <c:v>74061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300206</c:v>
+                  <c:v>301906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2563819</c:v>
+                  <c:v>2580819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27128,7 +27128,7 @@
                   <c:v>67487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59329</c:v>
+                  <c:v>57239</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>52378</c:v>
@@ -51764,7 +51764,7 @@
   <dimension ref="C3:AC37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -51828,13 +51828,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>74559</v>
+        <v>74788</v>
       </c>
       <c r="K4" s="4">
-        <v>305347</v>
+        <v>307637</v>
       </c>
       <c r="L4" s="4">
-        <v>2613690</v>
+        <v>2636590</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -51867,10 +51867,10 @@
         <v>3</v>
       </c>
       <c r="J5" s="4">
-        <v>60149</v>
+        <v>58022</v>
       </c>
       <c r="K5" s="5">
-        <v>64949</v>
+        <v>62822</v>
       </c>
       <c r="L5" s="4"/>
       <c r="O5" s="2" t="s">
@@ -51878,15 +51878,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>74559</v>
+        <v>74788</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>305347</v>
+        <v>307637</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2613690</v>
+        <v>2636590</v>
       </c>
     </row>
     <row r="6" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -51904,10 +51904,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>60364</v>
+        <v>58237</v>
       </c>
       <c r="K6" s="5">
-        <v>65164</v>
+        <v>63037</v>
       </c>
       <c r="L6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -51942,10 +51942,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
-        <v>207212</v>
+        <v>187607</v>
       </c>
       <c r="L7" s="5">
-        <v>212012</v>
+        <v>192407</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>11</v>
@@ -51976,10 +51976,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
-        <v>209141</v>
+        <v>189536</v>
       </c>
       <c r="L8" s="5">
-        <v>213941</v>
+        <v>194336</v>
       </c>
     </row>
     <row r="9" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -51997,7 +51997,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
-        <v>1258333</v>
+        <v>1197308</v>
       </c>
     </row>
     <row r="10" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52015,7 +52015,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>1267993</v>
+        <v>1206968</v>
       </c>
     </row>
     <row r="11" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52125,7 +52125,7 @@
       </c>
       <c r="P15" s="4">
         <f>J5</f>
-        <v>60149</v>
+        <v>58022</v>
       </c>
       <c r="Q15"/>
       <c r="R15"/>
@@ -52134,7 +52134,7 @@
       </c>
       <c r="Z15" s="4">
         <f>J6</f>
-        <v>60364</v>
+        <v>58237</v>
       </c>
     </row>
     <row r="16" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52347,22 +52347,22 @@
       </c>
       <c r="P25" s="7">
         <f>K5</f>
-        <v>64949</v>
+        <v>62822</v>
       </c>
       <c r="Q25" s="4">
         <f>K7</f>
-        <v>207212</v>
+        <v>187607</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z25" s="7">
         <f>K6</f>
-        <v>65164</v>
+        <v>63037</v>
       </c>
       <c r="AA25" s="4">
         <f>K8</f>
-        <v>209141</v>
+        <v>189536</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52463,22 +52463,22 @@
       </c>
       <c r="P35" s="7">
         <f>L7</f>
-        <v>212012</v>
+        <v>192407</v>
       </c>
       <c r="Q35" s="4">
         <f>L10</f>
-        <v>1267993</v>
+        <v>1206968</v>
       </c>
       <c r="Y35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z35" s="7">
         <f>L8</f>
-        <v>213941</v>
+        <v>194336</v>
       </c>
       <c r="AA35" s="4">
         <f>L10</f>
-        <v>1267993</v>
+        <v>1206968</v>
       </c>
     </row>
     <row r="36" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52540,8 +52540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A4B072-C80B-4A23-A0B3-8E3559BB66E3}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52604,13 +52604,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>73891</v>
+        <v>74061</v>
       </c>
       <c r="K4" s="4">
-        <v>300206</v>
+        <v>301906</v>
       </c>
       <c r="L4" s="4">
-        <v>2563819</v>
+        <v>2580819</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -52643,10 +52643,10 @@
         <v>3</v>
       </c>
       <c r="J5" s="4">
-        <v>59329</v>
+        <v>57239</v>
       </c>
       <c r="K5" s="5">
-        <v>64129</v>
+        <v>62039</v>
       </c>
       <c r="L5" s="4"/>
       <c r="O5" s="2" t="s">
@@ -52654,15 +52654,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>73891</v>
+        <v>74061</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>300206</v>
+        <v>301906</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2563819</v>
+        <v>2580819</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52680,10 +52680,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>59398</v>
+        <v>57308</v>
       </c>
       <c r="K6" s="5">
-        <v>64198</v>
+        <v>62108</v>
       </c>
       <c r="L6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -52718,10 +52718,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
-        <v>196776</v>
+        <v>175741</v>
       </c>
       <c r="L7" s="5">
-        <v>201576</v>
+        <v>180541</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>11</v>
@@ -52752,10 +52752,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
-        <v>196255</v>
+        <v>175220</v>
       </c>
       <c r="L8" s="5">
-        <v>201055</v>
+        <v>180020</v>
       </c>
     </row>
     <row r="9" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52773,7 +52773,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
-        <v>1129757</v>
+        <v>1021582</v>
       </c>
     </row>
     <row r="10" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52791,7 +52791,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>1105167</v>
+        <v>996992</v>
       </c>
     </row>
     <row r="11" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52900,7 +52900,7 @@
       </c>
       <c r="P15" s="4">
         <f>J5</f>
-        <v>59329</v>
+        <v>57239</v>
       </c>
       <c r="Q15"/>
       <c r="Y15" s="2" t="s">
@@ -52908,7 +52908,7 @@
       </c>
       <c r="Z15" s="4">
         <f>J6</f>
-        <v>59398</v>
+        <v>57308</v>
       </c>
       <c r="AA15"/>
     </row>
@@ -53127,22 +53127,22 @@
       </c>
       <c r="P25" s="7">
         <f>K5</f>
-        <v>64129</v>
+        <v>62039</v>
       </c>
       <c r="Q25" s="4">
         <f>K7</f>
-        <v>196776</v>
+        <v>175741</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z25" s="7">
         <f>K6</f>
-        <v>64198</v>
+        <v>62108</v>
       </c>
       <c r="AA25" s="4">
         <f>K8</f>
-        <v>196255</v>
+        <v>175220</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53258,22 +53258,22 @@
       </c>
       <c r="P35" s="7">
         <f>L7</f>
-        <v>201576</v>
+        <v>180541</v>
       </c>
       <c r="Q35" s="4">
         <f>L10</f>
-        <v>1105167</v>
+        <v>996992</v>
       </c>
       <c r="Y35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z35" s="7">
         <f>L8</f>
-        <v>201055</v>
+        <v>180020</v>
       </c>
       <c r="AA35" s="4">
         <f>L10</f>
-        <v>1105167</v>
+        <v>996992</v>
       </c>
     </row>
     <row r="36" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53334,8 +53334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE8ECB1-BB77-4268-B40B-9743FF1BA452}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53398,13 +53398,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>73879</v>
+        <v>74049</v>
       </c>
       <c r="K4" s="4">
-        <v>300086</v>
+        <v>301786</v>
       </c>
       <c r="L4" s="4">
-        <v>2562619</v>
+        <v>2579619</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -53437,10 +53437,10 @@
         <v>3</v>
       </c>
       <c r="J5" s="4">
-        <v>59305</v>
+        <v>57227</v>
       </c>
       <c r="K5" s="5">
-        <v>64105</v>
+        <v>62027</v>
       </c>
       <c r="L5" s="4"/>
       <c r="O5" s="2" t="s">
@@ -53448,15 +53448,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>73879</v>
+        <v>74049</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>300086</v>
+        <v>301786</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2562619</v>
+        <v>2579619</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53474,10 +53474,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="4">
-        <v>59374</v>
+        <v>57296</v>
       </c>
       <c r="K6" s="5">
-        <v>64174</v>
+        <v>62096</v>
       </c>
       <c r="L6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -53512,10 +53512,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
-        <v>196536</v>
+        <v>175621</v>
       </c>
       <c r="L7" s="5">
-        <v>201336</v>
+        <v>180421</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>11</v>
@@ -53546,10 +53546,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
-        <v>196015</v>
+        <v>175100</v>
       </c>
       <c r="L8" s="5">
-        <v>200815</v>
+        <v>179900</v>
       </c>
     </row>
     <row r="9" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53567,7 +53567,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5">
-        <v>1128557</v>
+        <v>1020982</v>
       </c>
     </row>
     <row r="10" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53585,7 +53585,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>1103967</v>
+        <v>996392</v>
       </c>
     </row>
     <row r="11" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53694,7 +53694,7 @@
       </c>
       <c r="P15" s="4">
         <f>J5</f>
-        <v>59305</v>
+        <v>57227</v>
       </c>
       <c r="Q15"/>
       <c r="Y15" s="2" t="s">
@@ -53702,7 +53702,7 @@
       </c>
       <c r="Z15" s="4">
         <f>J6</f>
-        <v>59374</v>
+        <v>57296</v>
       </c>
       <c r="AA15"/>
     </row>
@@ -53921,22 +53921,22 @@
       </c>
       <c r="P25" s="7">
         <f>K5</f>
-        <v>64105</v>
+        <v>62027</v>
       </c>
       <c r="Q25" s="4">
         <f>K7</f>
-        <v>196536</v>
+        <v>175621</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z25" s="7">
         <f>K6</f>
-        <v>64174</v>
+        <v>62096</v>
       </c>
       <c r="AA25" s="4">
         <f>K8</f>
-        <v>196015</v>
+        <v>175100</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54052,22 +54052,22 @@
       </c>
       <c r="P35" s="7">
         <f>L7</f>
-        <v>201336</v>
+        <v>180421</v>
       </c>
       <c r="Q35" s="4">
         <f>L10</f>
-        <v>1103967</v>
+        <v>996392</v>
       </c>
       <c r="Y35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z35" s="7">
         <f>L8</f>
-        <v>200815</v>
+        <v>179900</v>
       </c>
       <c r="AA35" s="4">
         <f>L10</f>
-        <v>1103967</v>
+        <v>996392</v>
       </c>
     </row>
     <row r="36" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ERC721Enumerable data with latest OpenZeppelin version
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B737971-91EE-42E2-A971-F7970E9D7D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A14B410-EA03-47F3-A89E-0E7B69992729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
@@ -513,13 +513,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>124202</c:v>
+                  <c:v>124478</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1159927</c:v>
+                  <c:v>1162687</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11517332</c:v>
+                  <c:v>11544932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1369,7 +1369,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>92881</c:v>
+                  <c:v>90830</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62039</c:v>
@@ -1469,7 +1469,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>442480</c:v>
+                  <c:v>421970</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175741</c:v>
@@ -2011,7 +2011,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>557550</c:v>
+                  <c:v>537040</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180541</c:v>
@@ -2111,7 +2111,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2939851</c:v>
+                  <c:v>2837301</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996992</c:v>
@@ -2662,7 +2662,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67468</c:v>
+                  <c:v>65417</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57308</c:v>
@@ -3224,7 +3224,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>88168</c:v>
+                  <c:v>86117</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62108</c:v>
@@ -3324,7 +3324,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>460624</c:v>
+                  <c:v>440114</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175220</c:v>
@@ -3916,7 +3916,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>484889</c:v>
+                  <c:v>464379</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180020</c:v>
@@ -4016,7 +4016,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2543251</c:v>
+                  <c:v>2440701</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996992</c:v>
@@ -4560,13 +4560,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123275</c:v>
+                  <c:v>123481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1152268</c:v>
+                  <c:v>1154328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11442376</c:v>
+                  <c:v>11462976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5385,7 +5385,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67419</c:v>
+                  <c:v>65380</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57227</c:v>
@@ -5951,7 +5951,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>92813</c:v>
+                  <c:v>90774</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62027</c:v>
@@ -6051,7 +6051,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>442196</c:v>
+                  <c:v>421806</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175621</c:v>
@@ -6643,7 +6643,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>557266</c:v>
+                  <c:v>536876</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180421</c:v>
@@ -6743,7 +6743,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2938607</c:v>
+                  <c:v>2836657</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996392</c:v>
@@ -7285,7 +7285,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67467</c:v>
+                  <c:v>65428</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57296</c:v>
@@ -7824,7 +7824,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>68519</c:v>
+                  <c:v>66454</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>58022</c:v>
@@ -8349,7 +8349,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>88167</c:v>
+                  <c:v>86128</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62096</c:v>
@@ -8449,7 +8449,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>460340</c:v>
+                  <c:v>439950</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175100</c:v>
@@ -9004,7 +9004,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>484605</c:v>
+                  <c:v>464215</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>179900</c:v>
@@ -9104,7 +9104,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2542051</c:v>
+                  <c:v>2440101</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996392</c:v>
@@ -9641,13 +9641,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>124202</c:v>
+                  <c:v>124478</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1159927</c:v>
+                  <c:v>1162687</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11517332</c:v>
+                  <c:v>11544932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10447,13 +10447,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123287</c:v>
+                  <c:v>123493</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1152388</c:v>
+                  <c:v>1154448</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11443553</c:v>
+                  <c:v>11464153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11262,13 +11262,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123275</c:v>
+                  <c:v>123481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1152268</c:v>
+                  <c:v>1154328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11442376</c:v>
+                  <c:v>11462976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12113,7 +12113,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>92881</c:v>
+                  <c:v>90830</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62039</c:v>
@@ -12213,7 +12213,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>442480</c:v>
+                  <c:v>421970</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175741</c:v>
@@ -12760,7 +12760,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>94074</c:v>
+                  <c:v>92009</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62822</c:v>
@@ -12860,7 +12860,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>455841</c:v>
+                  <c:v>437126</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>187607</c:v>
@@ -13434,7 +13434,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>68519</c:v>
+                  <c:v>66454</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>58022</c:v>
@@ -13967,7 +13967,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67487</c:v>
+                  <c:v>65436</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57239</c:v>
@@ -14484,7 +14484,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>571716</c:v>
+                  <c:v>553001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>192407</c:v>
@@ -14584,7 +14584,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3087077</c:v>
+                  <c:v>3036502</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1206968</c:v>
@@ -15126,7 +15126,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>94074</c:v>
+                  <c:v>92009</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62822</c:v>
@@ -15226,7 +15226,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>455841</c:v>
+                  <c:v>437126</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>187607</c:v>
@@ -15785,7 +15785,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>557550</c:v>
+                  <c:v>537040</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180541</c:v>
@@ -15885,7 +15885,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2939851</c:v>
+                  <c:v>2837301</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996992</c:v>
@@ -16451,7 +16451,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67419</c:v>
+                  <c:v>65380</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57227</c:v>
@@ -16994,7 +16994,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>92813</c:v>
+                  <c:v>90774</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62027</c:v>
@@ -17094,7 +17094,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>442196</c:v>
+                  <c:v>421806</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175621</c:v>
@@ -17663,7 +17663,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>557266</c:v>
+                  <c:v>536876</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180421</c:v>
@@ -17763,7 +17763,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2938607</c:v>
+                  <c:v>2836657</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996392</c:v>
@@ -18309,7 +18309,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>68646</c:v>
+                  <c:v>66581</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>58237</c:v>
@@ -18830,7 +18830,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>89346</c:v>
+                  <c:v>87281</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>63037</c:v>
@@ -18930,7 +18930,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>476033</c:v>
+                  <c:v>457318</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>189536</c:v>
@@ -19476,7 +19476,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>499895</c:v>
+                  <c:v>481180</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>194336</c:v>
@@ -19576,7 +19576,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2716677</c:v>
+                  <c:v>2666102</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1206968</c:v>
@@ -20128,7 +20128,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67468</c:v>
+                  <c:v>65417</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57308</c:v>
@@ -20667,7 +20667,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>88168</c:v>
+                  <c:v>86117</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62108</c:v>
@@ -20767,7 +20767,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>460624</c:v>
+                  <c:v>440114</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175220</c:v>
@@ -21336,7 +21336,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>484889</c:v>
+                  <c:v>464379</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180020</c:v>
@@ -21436,7 +21436,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2543251</c:v>
+                  <c:v>2440701</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996992</c:v>
@@ -21983,7 +21983,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>571716</c:v>
+                  <c:v>553001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>192407</c:v>
@@ -22083,7 +22083,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3087077</c:v>
+                  <c:v>3036502</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1206968</c:v>
@@ -22627,7 +22627,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67467</c:v>
+                  <c:v>65428</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57296</c:v>
@@ -23149,7 +23149,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>88167</c:v>
+                  <c:v>86128</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>62096</c:v>
@@ -23249,7 +23249,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>460340</c:v>
+                  <c:v>439950</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>175100</c:v>
@@ -23801,7 +23801,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>484605</c:v>
+                  <c:v>464215</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>179900</c:v>
@@ -23901,7 +23901,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2542051</c:v>
+                  <c:v>2440101</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>996392</c:v>
@@ -24447,7 +24447,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>68646</c:v>
+                  <c:v>66581</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>58237</c:v>
@@ -24991,7 +24991,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>89346</c:v>
+                  <c:v>87281</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>63037</c:v>
@@ -25091,7 +25091,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>476033</c:v>
+                  <c:v>457318</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>189536</c:v>
@@ -25660,7 +25660,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>499895</c:v>
+                  <c:v>481180</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>194336</c:v>
@@ -25760,7 +25760,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2716677</c:v>
+                  <c:v>2666102</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1206968</c:v>
@@ -26300,13 +26300,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123287</c:v>
+                  <c:v>123493</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1152388</c:v>
+                  <c:v>1154448</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11443553</c:v>
+                  <c:v>11464153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27125,7 +27125,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67487</c:v>
+                  <c:v>65436</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57239</c:v>
@@ -51764,7 +51764,7 @@
   <dimension ref="C3:AC37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -51816,13 +51816,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>124202</v>
+        <v>124478</v>
       </c>
       <c r="E4" s="4">
-        <v>1159927</v>
+        <v>1162687</v>
       </c>
       <c r="F4" s="4">
-        <v>11517332</v>
+        <v>11544932</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -51841,15 +51841,15 @@
       </c>
       <c r="P4" s="4">
         <f>D4</f>
-        <v>124202</v>
+        <v>124478</v>
       </c>
       <c r="Q4" s="4">
         <f>E4</f>
-        <v>1159927</v>
+        <v>1162687</v>
       </c>
       <c r="R4" s="4">
         <f>F4</f>
-        <v>11517332</v>
+        <v>11544932</v>
       </c>
     </row>
     <row r="5" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -51857,10 +51857,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="4">
-        <v>68519</v>
+        <v>66454</v>
       </c>
       <c r="E5" s="5">
-        <v>94074</v>
+        <v>92009</v>
       </c>
       <c r="F5" s="4"/>
       <c r="I5" s="3" t="s">
@@ -51894,10 +51894,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>68646</v>
+        <v>66581</v>
       </c>
       <c r="E6" s="5">
-        <v>89346</v>
+        <v>87281</v>
       </c>
       <c r="F6" s="4"/>
       <c r="I6" s="3" t="s">
@@ -51932,10 +51932,10 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>455841</v>
+        <v>437126</v>
       </c>
       <c r="F7" s="5">
-        <v>571716</v>
+        <v>553001</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>5</v>
@@ -51966,10 +51966,10 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
-        <v>476033</v>
+        <v>457318</v>
       </c>
       <c r="F8" s="5">
-        <v>499895</v>
+        <v>481180</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>6</v>
@@ -51989,7 +51989,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5">
-        <v>3087077</v>
+        <v>3036502</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>7</v>
@@ -52007,7 +52007,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5">
-        <v>2716677</v>
+        <v>2666102</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>8</v>
@@ -52083,7 +52083,7 @@
       </c>
       <c r="P14" s="4">
         <f>D5</f>
-        <v>68519</v>
+        <v>66454</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
@@ -52092,7 +52092,7 @@
       </c>
       <c r="Z14" s="4">
         <f>D6</f>
-        <v>68646</v>
+        <v>66581</v>
       </c>
     </row>
     <row r="15" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52323,22 +52323,22 @@
       </c>
       <c r="P24" s="7">
         <f>E5</f>
-        <v>94074</v>
+        <v>92009</v>
       </c>
       <c r="Q24" s="4">
         <f>E7</f>
-        <v>455841</v>
+        <v>437126</v>
       </c>
       <c r="Y24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Z24" s="7">
         <f>E6</f>
-        <v>89346</v>
+        <v>87281</v>
       </c>
       <c r="AA24" s="4">
         <f>E8</f>
-        <v>476033</v>
+        <v>457318</v>
       </c>
     </row>
     <row r="25" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52439,22 +52439,22 @@
       </c>
       <c r="P34" s="7">
         <f>F7</f>
-        <v>571716</v>
+        <v>553001</v>
       </c>
       <c r="Q34" s="4">
         <f>F9</f>
-        <v>3087077</v>
+        <v>3036502</v>
       </c>
       <c r="Y34" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Z34" s="7">
         <f>F8</f>
-        <v>499895</v>
+        <v>481180</v>
       </c>
       <c r="AA34" s="4">
         <f>F10</f>
-        <v>2716677</v>
+        <v>2666102</v>
       </c>
     </row>
     <row r="35" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52541,7 +52541,7 @@
   <dimension ref="C3:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52592,13 +52592,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>123287</v>
+        <v>123493</v>
       </c>
       <c r="E4" s="4">
-        <v>1152388</v>
+        <v>1154448</v>
       </c>
       <c r="F4" s="4">
-        <v>11443553</v>
+        <v>11464153</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -52617,15 +52617,15 @@
       </c>
       <c r="P4" s="4">
         <f>D4</f>
-        <v>123287</v>
+        <v>123493</v>
       </c>
       <c r="Q4" s="4">
         <f>E4</f>
-        <v>1152388</v>
+        <v>1154448</v>
       </c>
       <c r="R4" s="4">
         <f>F4</f>
-        <v>11443553</v>
+        <v>11464153</v>
       </c>
     </row>
     <row r="5" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52633,10 +52633,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="4">
-        <v>67487</v>
+        <v>65436</v>
       </c>
       <c r="E5" s="5">
-        <v>92881</v>
+        <v>90830</v>
       </c>
       <c r="F5" s="4"/>
       <c r="I5" s="3" t="s">
@@ -52670,10 +52670,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>67468</v>
+        <v>65417</v>
       </c>
       <c r="E6" s="5">
-        <v>88168</v>
+        <v>86117</v>
       </c>
       <c r="F6" s="4"/>
       <c r="I6" s="3" t="s">
@@ -52708,10 +52708,10 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>442480</v>
+        <v>421970</v>
       </c>
       <c r="F7" s="5">
-        <v>557550</v>
+        <v>537040</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>5</v>
@@ -52742,10 +52742,10 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
-        <v>460624</v>
+        <v>440114</v>
       </c>
       <c r="F8" s="5">
-        <v>484889</v>
+        <v>464379</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>6</v>
@@ -52765,7 +52765,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5">
-        <v>2939851</v>
+        <v>2837301</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>7</v>
@@ -52783,7 +52783,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5">
-        <v>2543251</v>
+        <v>2440701</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>8</v>
@@ -52858,7 +52858,7 @@
       </c>
       <c r="P14" s="4">
         <f>D5</f>
-        <v>67487</v>
+        <v>65436</v>
       </c>
       <c r="Q14"/>
       <c r="Y14" s="2" t="s">
@@ -52866,7 +52866,7 @@
       </c>
       <c r="Z14" s="4">
         <f>D6</f>
-        <v>67468</v>
+        <v>65417</v>
       </c>
       <c r="AA14"/>
     </row>
@@ -53103,22 +53103,22 @@
       </c>
       <c r="P24" s="7">
         <f>E5</f>
-        <v>92881</v>
+        <v>90830</v>
       </c>
       <c r="Q24" s="4">
         <f>E7</f>
-        <v>442480</v>
+        <v>421970</v>
       </c>
       <c r="Y24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Z24" s="7">
         <f>E6</f>
-        <v>88168</v>
+        <v>86117</v>
       </c>
       <c r="AA24" s="4">
         <f>E8</f>
-        <v>460624</v>
+        <v>440114</v>
       </c>
     </row>
     <row r="25" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53234,22 +53234,22 @@
       </c>
       <c r="P34" s="7">
         <f>F7</f>
-        <v>557550</v>
+        <v>537040</v>
       </c>
       <c r="Q34" s="4">
         <f>F9</f>
-        <v>2939851</v>
+        <v>2837301</v>
       </c>
       <c r="Y34" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Z34" s="7">
         <f>F8</f>
-        <v>484889</v>
+        <v>464379</v>
       </c>
       <c r="AA34" s="4">
         <f>F10</f>
-        <v>2543251</v>
+        <v>2440701</v>
       </c>
     </row>
     <row r="35" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53335,7 +53335,7 @@
   <dimension ref="C3:AA37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53386,13 +53386,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>123275</v>
+        <v>123481</v>
       </c>
       <c r="E4" s="4">
-        <v>1152268</v>
+        <v>1154328</v>
       </c>
       <c r="F4" s="4">
-        <v>11442376</v>
+        <v>11462976</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -53411,15 +53411,15 @@
       </c>
       <c r="P4" s="4">
         <f>D4</f>
-        <v>123275</v>
+        <v>123481</v>
       </c>
       <c r="Q4" s="4">
         <f>E4</f>
-        <v>1152268</v>
+        <v>1154328</v>
       </c>
       <c r="R4" s="4">
         <f>F4</f>
-        <v>11442376</v>
+        <v>11462976</v>
       </c>
     </row>
     <row r="5" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53427,10 +53427,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="4">
-        <v>67419</v>
+        <v>65380</v>
       </c>
       <c r="E5" s="5">
-        <v>92813</v>
+        <v>90774</v>
       </c>
       <c r="F5" s="4"/>
       <c r="I5" s="3" t="s">
@@ -53464,10 +53464,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>67467</v>
+        <v>65428</v>
       </c>
       <c r="E6" s="5">
-        <v>88167</v>
+        <v>86128</v>
       </c>
       <c r="F6" s="4"/>
       <c r="I6" s="3" t="s">
@@ -53502,10 +53502,10 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>442196</v>
+        <v>421806</v>
       </c>
       <c r="F7" s="5">
-        <v>557266</v>
+        <v>536876</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>5</v>
@@ -53536,10 +53536,10 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
-        <v>460340</v>
+        <v>439950</v>
       </c>
       <c r="F8" s="5">
-        <v>484605</v>
+        <v>464215</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>6</v>
@@ -53559,7 +53559,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5">
-        <v>2938607</v>
+        <v>2836657</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>7</v>
@@ -53577,7 +53577,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5">
-        <v>2542051</v>
+        <v>2440101</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>8</v>
@@ -53652,7 +53652,7 @@
       </c>
       <c r="P14" s="4">
         <f>D5</f>
-        <v>67419</v>
+        <v>65380</v>
       </c>
       <c r="Q14"/>
       <c r="Y14" s="2" t="s">
@@ -53660,7 +53660,7 @@
       </c>
       <c r="Z14" s="4">
         <f>D6</f>
-        <v>67467</v>
+        <v>65428</v>
       </c>
       <c r="AA14"/>
     </row>
@@ -53897,22 +53897,22 @@
       </c>
       <c r="P24" s="7">
         <f>E5</f>
-        <v>92813</v>
+        <v>90774</v>
       </c>
       <c r="Q24" s="4">
         <f>E7</f>
-        <v>442196</v>
+        <v>421806</v>
       </c>
       <c r="Y24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Z24" s="7">
         <f>E6</f>
-        <v>88167</v>
+        <v>86128</v>
       </c>
       <c r="AA24" s="4">
         <f>E8</f>
-        <v>460340</v>
+        <v>439950</v>
       </c>
     </row>
     <row r="25" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54028,22 +54028,22 @@
       </c>
       <c r="P34" s="7">
         <f>F7</f>
-        <v>557266</v>
+        <v>536876</v>
       </c>
       <c r="Q34" s="4">
         <f>F9</f>
-        <v>2938607</v>
+        <v>2836657</v>
       </c>
       <c r="Y34" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Z34" s="7">
         <f>F8</f>
-        <v>484605</v>
+        <v>464215</v>
       </c>
       <c r="AA34" s="4">
         <f>F10</f>
-        <v>2542051</v>
+        <v>2440101</v>
       </c>
     </row>
     <row r="35" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ERC721F data with new mint loop
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A14B410-EA03-47F3-A89E-0E7B69992729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC51323-B889-46B7-BA6B-CCBD5E9C1C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled" sheetId="1" r:id="rId1"/>
@@ -607,13 +607,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74788</c:v>
+                  <c:v>74600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>307637</c:v>
+                  <c:v>305757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2636590</c:v>
+                  <c:v>2617790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4654,13 +4654,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74049</c:v>
+                  <c:v>73988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>301786</c:v>
+                  <c:v>301176</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2579619</c:v>
+                  <c:v>2573519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9735,13 +9735,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74788</c:v>
+                  <c:v>74600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>307637</c:v>
+                  <c:v>305757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2636590</c:v>
+                  <c:v>2617790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10541,13 +10541,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74061</c:v>
+                  <c:v>74000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>301906</c:v>
+                  <c:v>301296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2580819</c:v>
+                  <c:v>2574719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11356,13 +11356,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74049</c:v>
+                  <c:v>73988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>301786</c:v>
+                  <c:v>301176</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2579619</c:v>
+                  <c:v>2573519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26394,13 +26394,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74061</c:v>
+                  <c:v>74000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>301906</c:v>
+                  <c:v>301296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2580819</c:v>
+                  <c:v>2574719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -51764,7 +51764,7 @@
   <dimension ref="C3:AC37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -51828,13 +51828,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>74788</v>
+        <v>74600</v>
       </c>
       <c r="K4" s="4">
-        <v>307637</v>
+        <v>305757</v>
       </c>
       <c r="L4" s="4">
-        <v>2636590</v>
+        <v>2617790</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -51878,15 +51878,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>74788</v>
+        <v>74600</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>307637</v>
+        <v>305757</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2636590</v>
+        <v>2617790</v>
       </c>
     </row>
     <row r="6" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52540,8 +52540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A4B072-C80B-4A23-A0B3-8E3559BB66E3}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52604,13 +52604,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>74061</v>
+        <v>74000</v>
       </c>
       <c r="K4" s="4">
-        <v>301906</v>
+        <v>301296</v>
       </c>
       <c r="L4" s="4">
-        <v>2580819</v>
+        <v>2574719</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -52654,15 +52654,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>74061</v>
+        <v>74000</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>301906</v>
+        <v>301296</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2580819</v>
+        <v>2574719</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53334,8 +53334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE8ECB1-BB77-4268-B40B-9743FF1BA452}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53398,13 +53398,13 @@
         <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>74049</v>
+        <v>73988</v>
       </c>
       <c r="K4" s="4">
-        <v>301786</v>
+        <v>301176</v>
       </c>
       <c r="L4" s="4">
-        <v>2579619</v>
+        <v>2573519</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>24</v>
@@ -53448,15 +53448,15 @@
       </c>
       <c r="P5" s="4">
         <f>J4</f>
-        <v>74049</v>
+        <v>73988</v>
       </c>
       <c r="Q5" s="4">
         <f>K4</f>
-        <v>301786</v>
+        <v>301176</v>
       </c>
       <c r="R5" s="4">
         <f>L4</f>
-        <v>2579619</v>
+        <v>2573519</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ERC721Enumerable data with new mint loop
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC51323-B889-46B7-BA6B-CCBD5E9C1C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BA68E-6D35-4234-8D6C-CBDA32CA4871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
@@ -513,13 +513,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>124478</c:v>
+                  <c:v>124290</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1162687</c:v>
+                  <c:v>1160807</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11544932</c:v>
+                  <c:v>11526132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4560,13 +4560,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123481</c:v>
+                  <c:v>123420</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1154328</c:v>
+                  <c:v>1153718</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11462976</c:v>
+                  <c:v>11456876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9641,13 +9641,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>124478</c:v>
+                  <c:v>124290</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1162687</c:v>
+                  <c:v>1160807</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11544932</c:v>
+                  <c:v>11526132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10447,13 +10447,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123493</c:v>
+                  <c:v>123432</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1154448</c:v>
+                  <c:v>1153838</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11464153</c:v>
+                  <c:v>11458053</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11262,13 +11262,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123481</c:v>
+                  <c:v>123420</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1154328</c:v>
+                  <c:v>1153718</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11462976</c:v>
+                  <c:v>11456876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26300,13 +26300,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>123493</c:v>
+                  <c:v>123432</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1154448</c:v>
+                  <c:v>1153838</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11464153</c:v>
+                  <c:v>11458053</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -51764,7 +51764,7 @@
   <dimension ref="C3:AC37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -51816,13 +51816,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>124478</v>
+        <v>124290</v>
       </c>
       <c r="E4" s="4">
-        <v>1162687</v>
+        <v>1160807</v>
       </c>
       <c r="F4" s="4">
-        <v>11544932</v>
+        <v>11526132</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -51841,15 +51841,15 @@
       </c>
       <c r="P4" s="4">
         <f>D4</f>
-        <v>124478</v>
+        <v>124290</v>
       </c>
       <c r="Q4" s="4">
         <f>E4</f>
-        <v>1162687</v>
+        <v>1160807</v>
       </c>
       <c r="R4" s="4">
         <f>F4</f>
-        <v>11544932</v>
+        <v>11526132</v>
       </c>
     </row>
     <row r="5" spans="3:26" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52541,7 +52541,7 @@
   <dimension ref="C3:AA37"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52592,13 +52592,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>123493</v>
+        <v>123432</v>
       </c>
       <c r="E4" s="4">
-        <v>1154448</v>
+        <v>1153838</v>
       </c>
       <c r="F4" s="4">
-        <v>11464153</v>
+        <v>11458053</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -52617,15 +52617,15 @@
       </c>
       <c r="P4" s="4">
         <f>D4</f>
-        <v>123493</v>
+        <v>123432</v>
       </c>
       <c r="Q4" s="4">
         <f>E4</f>
-        <v>1154448</v>
+        <v>1153838</v>
       </c>
       <c r="R4" s="4">
         <f>F4</f>
-        <v>11464153</v>
+        <v>11458053</v>
       </c>
     </row>
     <row r="5" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53335,7 +53335,7 @@
   <dimension ref="C3:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53386,13 +53386,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>123481</v>
+        <v>123420</v>
       </c>
       <c r="E4" s="4">
-        <v>1154328</v>
+        <v>1153718</v>
       </c>
       <c r="F4" s="4">
-        <v>11462976</v>
+        <v>11456876</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -53411,15 +53411,15 @@
       </c>
       <c r="P4" s="4">
         <f>D4</f>
-        <v>123481</v>
+        <v>123420</v>
       </c>
       <c r="Q4" s="4">
         <f>E4</f>
-        <v>1154328</v>
+        <v>1153718</v>
       </c>
       <c r="R4" s="4">
         <f>F4</f>
-        <v>11462976</v>
+        <v>11456876</v>
       </c>
     </row>
     <row r="5" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ERC721A and TinyERC721 data
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721Enumerable - ERC721F - ERC721A - TinyERC721.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE8D7D2-01D3-428D-B934-9B4E3964C737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C767C30F-7481-4D1E-91DB-0B43B4F1165F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
@@ -1375,7 +1375,7 @@
                   <c:v>62039</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85719</c:v>
+                  <c:v>83613</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>59329</c:v>
@@ -1475,7 +1475,7 @@
                   <c:v>175741</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247368</c:v>
+                  <c:v>244308</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>271011</c:v>
@@ -2017,7 +2017,7 @@
                   <c:v>180541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>358710</c:v>
+                  <c:v>355650</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>370994</c:v>
@@ -2117,7 +2117,7 @@
                   <c:v>993842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1936029</c:v>
+                  <c:v>1928729</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2510253</c:v>
@@ -2668,10 +2668,10 @@
                   <c:v>57245</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52403</c:v>
+                  <c:v>50234</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37077</c:v>
+                  <c:v>37014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3230,10 +3230,10 @@
                   <c:v>62045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104737</c:v>
+                  <c:v>102568</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76353</c:v>
+                  <c:v>76290</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3330,10 +3330,10 @@
                   <c:v>174590</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>255878</c:v>
+                  <c:v>252188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>280174</c:v>
+                  <c:v>279544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3922,10 +3922,10 @@
                   <c:v>179390</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>927901</c:v>
+                  <c:v>924211</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>982264</c:v>
+                  <c:v>981634</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4022,10 +4022,10 @@
                   <c:v>993842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3554711</c:v>
+                  <c:v>3544261</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4300654</c:v>
+                  <c:v>4297504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5391,10 +5391,10 @@
                   <c:v>57227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52401</c:v>
+                  <c:v>50295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37051</c:v>
+                  <c:v>37029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5957,7 +5957,7 @@
                   <c:v>62027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85742</c:v>
+                  <c:v>83636</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>59328</c:v>
@@ -6057,7 +6057,7 @@
                   <c:v>175621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247324</c:v>
+                  <c:v>244264</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>270749</c:v>
@@ -6649,7 +6649,7 @@
                   <c:v>180421</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>358666</c:v>
+                  <c:v>355606</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>370732</c:v>
@@ -6749,7 +6749,7 @@
                   <c:v>993242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1935985</c:v>
+                  <c:v>1928685</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2509009</c:v>
@@ -7291,10 +7291,10 @@
                   <c:v>57233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52426</c:v>
+                  <c:v>50257</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37076</c:v>
+                  <c:v>36991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7830,7 +7830,7 @@
                   <c:v>58022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53288</c:v>
+                  <c:v>51182</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38399</c:v>
@@ -8355,10 +8355,10 @@
                   <c:v>62033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104760</c:v>
+                  <c:v>102591</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76352</c:v>
+                  <c:v>76289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8455,10 +8455,10 @@
                   <c:v>174470</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>255834</c:v>
+                  <c:v>252144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>279890</c:v>
+                  <c:v>279260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9010,10 +9010,10 @@
                   <c:v>179270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>927857</c:v>
+                  <c:v>924167</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>981980</c:v>
+                  <c:v>981350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9110,10 +9110,10 @@
                   <c:v>993242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3554667</c:v>
+                  <c:v>3544217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4299410</c:v>
+                  <c:v>4296260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12119,7 +12119,7 @@
                   <c:v>62039</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85719</c:v>
+                  <c:v>83613</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>59329</c:v>
@@ -12219,7 +12219,7 @@
                   <c:v>175741</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247368</c:v>
+                  <c:v>244308</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>271011</c:v>
@@ -12766,7 +12766,7 @@
                   <c:v>62822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86676</c:v>
+                  <c:v>84570</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>61184</c:v>
@@ -12866,7 +12866,7 @@
                   <c:v>187607</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260100</c:v>
+                  <c:v>257040</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>293377</c:v>
@@ -13440,7 +13440,7 @@
                   <c:v>58022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53288</c:v>
+                  <c:v>51182</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38399</c:v>
@@ -13973,7 +13973,7 @@
                   <c:v>57239</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52378</c:v>
+                  <c:v>50272</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>37052</c:v>
@@ -14490,7 +14490,7 @@
                   <c:v>192407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>371686</c:v>
+                  <c:v>368626</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>395875</c:v>
@@ -14590,7 +14590,7 @@
                   <c:v>1197868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2103305</c:v>
+                  <c:v>2096005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2802054</c:v>
@@ -15132,7 +15132,7 @@
                   <c:v>62822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86676</c:v>
+                  <c:v>84570</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>61184</c:v>
@@ -15232,7 +15232,7 @@
                   <c:v>187607</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260100</c:v>
+                  <c:v>257040</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>293377</c:v>
@@ -15791,7 +15791,7 @@
                   <c:v>180541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>358710</c:v>
+                  <c:v>355650</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>370994</c:v>
@@ -15891,7 +15891,7 @@
                   <c:v>993842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1936029</c:v>
+                  <c:v>1928729</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2510253</c:v>
@@ -16457,10 +16457,10 @@
                   <c:v>57227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52401</c:v>
+                  <c:v>50295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37051</c:v>
+                  <c:v>37029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17000,7 +17000,7 @@
                   <c:v>62027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85742</c:v>
+                  <c:v>83636</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>59328</c:v>
@@ -17100,7 +17100,7 @@
                   <c:v>175621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247324</c:v>
+                  <c:v>244264</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>270749</c:v>
@@ -17669,7 +17669,7 @@
                   <c:v>180421</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>358666</c:v>
+                  <c:v>355606</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>370732</c:v>
@@ -17769,7 +17769,7 @@
                   <c:v>993242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1935985</c:v>
+                  <c:v>1928685</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2509009</c:v>
@@ -18315,10 +18315,10 @@
                   <c:v>58055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53459</c:v>
+                  <c:v>51171</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38570</c:v>
+                  <c:v>38388</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18836,10 +18836,10 @@
                   <c:v>62855</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>106591</c:v>
+                  <c:v>104303</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78962</c:v>
+                  <c:v>78780</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18936,10 +18936,10 @@
                   <c:v>187716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>272852</c:v>
+                  <c:v>267972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>305773</c:v>
+                  <c:v>303953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19482,10 +19482,10 @@
                   <c:v>192516</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1026068</c:v>
+                  <c:v>1021188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1122253</c:v>
+                  <c:v>1120433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19582,10 +19582,10 @@
                   <c:v>1197868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4081938</c:v>
+                  <c:v>4065538</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5066243</c:v>
+                  <c:v>5057143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20134,10 +20134,10 @@
                   <c:v>57245</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52403</c:v>
+                  <c:v>50234</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37077</c:v>
+                  <c:v>37014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20673,10 +20673,10 @@
                   <c:v>62045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104737</c:v>
+                  <c:v>102568</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76353</c:v>
+                  <c:v>76290</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20773,10 +20773,10 @@
                   <c:v>174590</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>255878</c:v>
+                  <c:v>252188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>280174</c:v>
+                  <c:v>279544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21342,10 +21342,10 @@
                   <c:v>179390</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>927901</c:v>
+                  <c:v>924211</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>982264</c:v>
+                  <c:v>981634</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21442,10 +21442,10 @@
                   <c:v>993842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3554711</c:v>
+                  <c:v>3544261</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4300654</c:v>
+                  <c:v>4297504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21989,7 +21989,7 @@
                   <c:v>192407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>371686</c:v>
+                  <c:v>368626</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>395875</c:v>
@@ -22089,7 +22089,7 @@
                   <c:v>1197868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2103305</c:v>
+                  <c:v>2096005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2802054</c:v>
@@ -22633,10 +22633,10 @@
                   <c:v>57233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52426</c:v>
+                  <c:v>50257</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37076</c:v>
+                  <c:v>36991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23155,10 +23155,10 @@
                   <c:v>62033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104760</c:v>
+                  <c:v>102591</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76352</c:v>
+                  <c:v>76289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23255,10 +23255,10 @@
                   <c:v>174470</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>255834</c:v>
+                  <c:v>252144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>279890</c:v>
+                  <c:v>279260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23807,10 +23807,10 @@
                   <c:v>179270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>927857</c:v>
+                  <c:v>924167</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>981980</c:v>
+                  <c:v>981350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23907,10 +23907,10 @@
                   <c:v>993242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3554667</c:v>
+                  <c:v>3544217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4299410</c:v>
+                  <c:v>4296260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24453,10 +24453,10 @@
                   <c:v>58055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53459</c:v>
+                  <c:v>51171</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38570</c:v>
+                  <c:v>38388</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24997,10 +24997,10 @@
                   <c:v>62855</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>106591</c:v>
+                  <c:v>104303</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78962</c:v>
+                  <c:v>78780</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25097,10 +25097,10 @@
                   <c:v>187716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>272852</c:v>
+                  <c:v>267972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>305773</c:v>
+                  <c:v>303953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25666,10 +25666,10 @@
                   <c:v>192516</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1026068</c:v>
+                  <c:v>1021188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1122253</c:v>
+                  <c:v>1120433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25766,10 +25766,10 @@
                   <c:v>1197868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4081938</c:v>
+                  <c:v>4065538</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5066243</c:v>
+                  <c:v>5057143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27131,7 +27131,7 @@
                   <c:v>57239</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52378</c:v>
+                  <c:v>50272</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>37052</c:v>
@@ -51764,7 +51764,7 @@
   <dimension ref="C3:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52142,10 +52142,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="4">
-        <v>53288</v>
+        <v>51182</v>
       </c>
       <c r="E16" s="5">
-        <v>86676</v>
+        <v>84570</v>
       </c>
       <c r="F16" s="4"/>
       <c r="I16" s="3" t="s">
@@ -52163,7 +52163,7 @@
       </c>
       <c r="P16" s="4">
         <f>D16</f>
-        <v>53288</v>
+        <v>51182</v>
       </c>
       <c r="Q16"/>
       <c r="R16"/>
@@ -52172,7 +52172,7 @@
       </c>
       <c r="Z16" s="4">
         <f>D17</f>
-        <v>53459</v>
+        <v>51171</v>
       </c>
     </row>
     <row r="17" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52180,20 +52180,20 @@
         <v>4</v>
       </c>
       <c r="D17" s="4">
-        <v>53459</v>
+        <v>51171</v>
       </c>
       <c r="E17" s="5">
-        <v>106591</v>
+        <v>104303</v>
       </c>
       <c r="F17" s="4"/>
       <c r="I17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="4">
-        <v>38570</v>
+        <v>38388</v>
       </c>
       <c r="K17" s="5">
-        <v>78962</v>
+        <v>78780</v>
       </c>
       <c r="L17" s="4"/>
       <c r="O17" s="2" t="s">
@@ -52210,7 +52210,7 @@
       </c>
       <c r="Z17" s="4">
         <f>J17</f>
-        <v>38570</v>
+        <v>38388</v>
       </c>
     </row>
     <row r="18" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52219,10 +52219,10 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
-        <v>260100</v>
+        <v>257040</v>
       </c>
       <c r="F18" s="5">
-        <v>371686</v>
+        <v>368626</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>5</v>
@@ -52243,20 +52243,20 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
-        <v>272852</v>
+        <v>267972</v>
       </c>
       <c r="F19" s="5">
-        <v>1026068</v>
+        <v>1021188</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4">
-        <v>305773</v>
+        <v>303953</v>
       </c>
       <c r="L19" s="5">
-        <v>1122253</v>
+        <v>1120433</v>
       </c>
       <c r="Q19"/>
       <c r="R19"/>
@@ -52268,7 +52268,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="5">
-        <v>2103305</v>
+        <v>2096005</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>7</v>
@@ -52286,7 +52286,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5">
-        <v>4081938</v>
+        <v>4065538</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>8</v>
@@ -52294,7 +52294,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="5">
-        <v>5066243</v>
+        <v>5057143</v>
       </c>
     </row>
     <row r="23" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52371,22 +52371,22 @@
       </c>
       <c r="P26" s="7">
         <f>E16</f>
-        <v>86676</v>
+        <v>84570</v>
       </c>
       <c r="Q26" s="4">
         <f>E18</f>
-        <v>260100</v>
+        <v>257040</v>
       </c>
       <c r="Y26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z26" s="7">
         <f>E17</f>
-        <v>106591</v>
+        <v>104303</v>
       </c>
       <c r="AA26" s="4">
         <f>E19</f>
-        <v>272852</v>
+        <v>267972</v>
       </c>
     </row>
     <row r="27" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52406,11 +52406,11 @@
       </c>
       <c r="Z27" s="7">
         <f>K17</f>
-        <v>78962</v>
+        <v>78780</v>
       </c>
       <c r="AA27" s="4">
         <f>K19</f>
-        <v>305773</v>
+        <v>303953</v>
       </c>
     </row>
     <row r="33" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52487,22 +52487,22 @@
       </c>
       <c r="P36" s="7">
         <f>F18</f>
-        <v>371686</v>
+        <v>368626</v>
       </c>
       <c r="Q36" s="4">
         <f>F20</f>
-        <v>2103305</v>
+        <v>2096005</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z36" s="7">
         <f>F19</f>
-        <v>1026068</v>
+        <v>1021188</v>
       </c>
       <c r="AA36" s="4">
         <f>F21</f>
-        <v>4081938</v>
+        <v>4065538</v>
       </c>
     </row>
     <row r="37" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -52522,11 +52522,11 @@
       </c>
       <c r="Z37" s="7">
         <f>L19</f>
-        <v>1122253</v>
+        <v>1120433</v>
       </c>
       <c r="AA37" s="4">
         <f>L21</f>
-        <v>5066243</v>
+        <v>5057143</v>
       </c>
     </row>
   </sheetData>
@@ -52540,8 +52540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A4B072-C80B-4A23-A0B3-8E3559BB66E3}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -52917,10 +52917,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="4">
-        <v>52378</v>
+        <v>50272</v>
       </c>
       <c r="E16" s="5">
-        <v>85719</v>
+        <v>83613</v>
       </c>
       <c r="F16" s="4"/>
       <c r="I16" s="3" t="s">
@@ -52938,7 +52938,7 @@
       </c>
       <c r="P16" s="4">
         <f>D16</f>
-        <v>52378</v>
+        <v>50272</v>
       </c>
       <c r="Q16"/>
       <c r="Y16" s="2" t="s">
@@ -52946,7 +52946,7 @@
       </c>
       <c r="Z16" s="4">
         <f>D17</f>
-        <v>52403</v>
+        <v>50234</v>
       </c>
       <c r="AA16"/>
     </row>
@@ -52955,20 +52955,20 @@
         <v>4</v>
       </c>
       <c r="D17" s="4">
-        <v>52403</v>
+        <v>50234</v>
       </c>
       <c r="E17" s="5">
-        <v>104737</v>
+        <v>102568</v>
       </c>
       <c r="F17" s="4"/>
       <c r="I17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="4">
-        <v>37077</v>
+        <v>37014</v>
       </c>
       <c r="K17" s="5">
-        <v>76353</v>
+        <v>76290</v>
       </c>
       <c r="L17" s="4"/>
       <c r="O17" s="2" t="s">
@@ -52984,7 +52984,7 @@
       </c>
       <c r="Z17" s="4">
         <f>J17</f>
-        <v>37077</v>
+        <v>37014</v>
       </c>
       <c r="AA17"/>
     </row>
@@ -52994,10 +52994,10 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
-        <v>247368</v>
+        <v>244308</v>
       </c>
       <c r="F18" s="5">
-        <v>358710</v>
+        <v>355650</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>5</v>
@@ -53018,20 +53018,20 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
-        <v>255878</v>
+        <v>252188</v>
       </c>
       <c r="F19" s="5">
-        <v>927901</v>
+        <v>924211</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4">
-        <v>280174</v>
+        <v>279544</v>
       </c>
       <c r="L19" s="5">
-        <v>982264</v>
+        <v>981634</v>
       </c>
       <c r="Q19"/>
       <c r="AA19"/>
@@ -53043,7 +53043,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="5">
-        <v>1936029</v>
+        <v>1928729</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>7</v>
@@ -53062,7 +53062,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5">
-        <v>3554711</v>
+        <v>3544261</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>8</v>
@@ -53070,7 +53070,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="5">
-        <v>4300654</v>
+        <v>4297504</v>
       </c>
       <c r="AA21"/>
     </row>
@@ -53151,22 +53151,22 @@
       </c>
       <c r="P26" s="7">
         <f>E16</f>
-        <v>85719</v>
+        <v>83613</v>
       </c>
       <c r="Q26" s="4">
         <f>E18</f>
-        <v>247368</v>
+        <v>244308</v>
       </c>
       <c r="Y26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z26" s="7">
         <f>E17</f>
-        <v>104737</v>
+        <v>102568</v>
       </c>
       <c r="AA26" s="4">
         <f>E19</f>
-        <v>255878</v>
+        <v>252188</v>
       </c>
     </row>
     <row r="27" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53186,11 +53186,11 @@
       </c>
       <c r="Z27" s="7">
         <f>K17</f>
-        <v>76353</v>
+        <v>76290</v>
       </c>
       <c r="AA27" s="4">
         <f>K19</f>
-        <v>280174</v>
+        <v>279544</v>
       </c>
     </row>
     <row r="28" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53282,22 +53282,22 @@
       </c>
       <c r="P36" s="7">
         <f>F18</f>
-        <v>358710</v>
+        <v>355650</v>
       </c>
       <c r="Q36" s="4">
         <f>F20</f>
-        <v>1936029</v>
+        <v>1928729</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z36" s="7">
         <f>F19</f>
-        <v>927901</v>
+        <v>924211</v>
       </c>
       <c r="AA36" s="4">
         <f>F21</f>
-        <v>3554711</v>
+        <v>3544261</v>
       </c>
     </row>
     <row r="37" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53317,11 +53317,11 @@
       </c>
       <c r="Z37" s="7">
         <f>L19</f>
-        <v>982264</v>
+        <v>981634</v>
       </c>
       <c r="AA37" s="4">
         <f>L21</f>
-        <v>4300654</v>
+        <v>4297504</v>
       </c>
     </row>
   </sheetData>
@@ -53334,8 +53334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE8ECB1-BB77-4268-B40B-9743FF1BA452}">
   <dimension ref="C3:AA37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53687,7 +53687,7 @@
         <v>78015</v>
       </c>
       <c r="L15" s="4">
-        <v>260018</v>
+        <v>259996</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>9</v>
@@ -53711,17 +53711,17 @@
         <v>3</v>
       </c>
       <c r="D16" s="4">
-        <v>52401</v>
+        <v>50295</v>
       </c>
       <c r="E16" s="5">
-        <v>85742</v>
+        <v>83636</v>
       </c>
       <c r="F16" s="4"/>
       <c r="I16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="4">
-        <v>37051</v>
+        <v>37029</v>
       </c>
       <c r="K16" s="5">
         <v>59328</v>
@@ -53732,7 +53732,7 @@
       </c>
       <c r="P16" s="4">
         <f>D16</f>
-        <v>52401</v>
+        <v>50295</v>
       </c>
       <c r="Q16"/>
       <c r="Y16" s="2" t="s">
@@ -53740,7 +53740,7 @@
       </c>
       <c r="Z16" s="4">
         <f>D17</f>
-        <v>52426</v>
+        <v>50257</v>
       </c>
       <c r="AA16"/>
     </row>
@@ -53749,20 +53749,20 @@
         <v>4</v>
       </c>
       <c r="D17" s="4">
-        <v>52426</v>
+        <v>50257</v>
       </c>
       <c r="E17" s="5">
-        <v>104760</v>
+        <v>102591</v>
       </c>
       <c r="F17" s="4"/>
       <c r="I17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="4">
-        <v>37076</v>
+        <v>36991</v>
       </c>
       <c r="K17" s="5">
-        <v>76352</v>
+        <v>76289</v>
       </c>
       <c r="L17" s="4"/>
       <c r="O17" s="2" t="s">
@@ -53770,7 +53770,7 @@
       </c>
       <c r="P17" s="4">
         <f>J16</f>
-        <v>37051</v>
+        <v>37029</v>
       </c>
       <c r="Q17"/>
       <c r="Y17" s="2" t="s">
@@ -53778,7 +53778,7 @@
       </c>
       <c r="Z17" s="4">
         <f>J17</f>
-        <v>37076</v>
+        <v>36991</v>
       </c>
       <c r="AA17"/>
     </row>
@@ -53788,10 +53788,10 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
-        <v>247324</v>
+        <v>244264</v>
       </c>
       <c r="F18" s="5">
-        <v>358666</v>
+        <v>355606</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>5</v>
@@ -53812,20 +53812,20 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
-        <v>255834</v>
+        <v>252144</v>
       </c>
       <c r="F19" s="5">
-        <v>927857</v>
+        <v>924167</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4">
-        <v>279890</v>
+        <v>279260</v>
       </c>
       <c r="L19" s="5">
-        <v>981980</v>
+        <v>981350</v>
       </c>
       <c r="Q19"/>
       <c r="AA19"/>
@@ -53837,7 +53837,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="5">
-        <v>1935985</v>
+        <v>1928685</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>7</v>
@@ -53856,7 +53856,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5">
-        <v>3554667</v>
+        <v>3544217</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>8</v>
@@ -53864,7 +53864,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="5">
-        <v>4299410</v>
+        <v>4296260</v>
       </c>
       <c r="AA21"/>
     </row>
@@ -53945,22 +53945,22 @@
       </c>
       <c r="P26" s="7">
         <f>E16</f>
-        <v>85742</v>
+        <v>83636</v>
       </c>
       <c r="Q26" s="4">
         <f>E18</f>
-        <v>247324</v>
+        <v>244264</v>
       </c>
       <c r="Y26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z26" s="7">
         <f>E17</f>
-        <v>104760</v>
+        <v>102591</v>
       </c>
       <c r="AA26" s="4">
         <f>E19</f>
-        <v>255834</v>
+        <v>252144</v>
       </c>
     </row>
     <row r="27" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -53980,11 +53980,11 @@
       </c>
       <c r="Z27" s="7">
         <f>K17</f>
-        <v>76352</v>
+        <v>76289</v>
       </c>
       <c r="AA27" s="4">
         <f>K19</f>
-        <v>279890</v>
+        <v>279260</v>
       </c>
     </row>
     <row r="28" spans="3:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54076,22 +54076,22 @@
       </c>
       <c r="P36" s="7">
         <f>F18</f>
-        <v>358666</v>
+        <v>355606</v>
       </c>
       <c r="Q36" s="4">
         <f>F20</f>
-        <v>1935985</v>
+        <v>1928685</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z36" s="7">
         <f>F19</f>
-        <v>927857</v>
+        <v>924167</v>
       </c>
       <c r="AA36" s="4">
         <f>F21</f>
-        <v>3554667</v>
+        <v>3544217</v>
       </c>
     </row>
     <row r="37" spans="15:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54111,11 +54111,11 @@
       </c>
       <c r="Z37" s="7">
         <f>L19</f>
-        <v>981980</v>
+        <v>981350</v>
       </c>
       <c r="AA37" s="4">
         <f>L21</f>
-        <v>4299410</v>
+        <v>4296260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>